<commit_message>
got the qualitative analysis running
</commit_message>
<xml_diff>
--- a/data/Guest Ambassador Rounding Survey.xlsx
+++ b/data/Guest Ambassador Rounding Survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandonchang/Desktop/medstar_volunteer_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C388F0A3-A077-D043-AED5-247261F8CE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEE06FE-7749-8246-A266-ACB568C40B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3618,8 +3618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A542" workbookViewId="0">
+      <selection activeCell="H550" sqref="H550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>